<commit_message>
Name changes and check interpolation
</commit_message>
<xml_diff>
--- a/edibles/utils/simulations/Charmi/fitting_6379_Alex/Compare_sightlines.xlsx
+++ b/edibles/utils/simulations/Charmi/fitting_6379_Alex/Compare_sightlines.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexr\edibles\edibles\utils\simulations\Charmi\fitting_6379_Alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F64D0-322E-429E-9C69-027AA6FC19E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3AECE8-4EC1-4D67-913E-4D3E9915177D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parallel_185859" sheetId="1" r:id="rId1"/>
     <sheet name="Perpendicular_185859" sheetId="2" r:id="rId2"/>
+    <sheet name="Parallel_all" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1526,7 +1527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1854,4 +1855,18 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64667688-5B82-49DB-83F1-B2C271367828}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified interpolation to reflect resolution
</commit_message>
<xml_diff>
--- a/edibles/utils/simulations/Charmi/fitting_6379_Alex/Compare_sightlines.xlsx
+++ b/edibles/utils/simulations/Charmi/fitting_6379_Alex/Compare_sightlines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexr\edibles\edibles\utils\simulations\Charmi\fitting_6379_Alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3AECE8-4EC1-4D67-913E-4D3E9915177D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDAC553-3D30-4E08-BD61-CD08CBB9A283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parallel_185859" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Parameters:</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Reduced chi square value</t>
+  </si>
+  <si>
+    <t>No. Observations co added</t>
   </si>
 </sst>
 </file>
@@ -660,13 +663,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>589486</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>1715699</xdr:rowOff>
@@ -1239,12 +1242,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{332CC4E6-F8F7-465C-998D-567A1C5FE01C}" name="Table2" displayName="Table2" ref="E5:G16" totalsRowShown="0">
-  <autoFilter ref="E5:G16" xr:uid="{332CC4E6-F8F7-465C-998D-567A1C5FE01C}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{332CC4E6-F8F7-465C-998D-567A1C5FE01C}" name="Table2" displayName="Table2" ref="E5:H16" totalsRowShown="0">
+  <autoFilter ref="E5:H16" xr:uid="{332CC4E6-F8F7-465C-998D-567A1C5FE01C}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{38778A02-0510-44BD-B1B6-AF5185538A0D}" name="Sightline" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{76F21CD0-A784-4C97-83BC-E93E37DE06BF}" name="Chi-Square" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{71FF0C84-6972-423D-AB9B-6717A7985248}" name="Plot"/>
+    <tableColumn id="4" xr3:uid="{00C94B05-AB9B-4219-8DE6-2947BFAAF43D}" name="No. Observations co added"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1525,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,19 +1540,20 @@
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.88671875" customWidth="1"/>
+    <col min="8" max="8" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1564,8 +1569,11 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="148.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="148.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1578,8 +1586,11 @@
       <c r="F6" s="1">
         <v>12.463539104218301</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1592,8 +1603,11 @@
       <c r="F7" s="1">
         <v>8.9321945775930391</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1606,8 +1620,11 @@
       <c r="F8" s="1">
         <v>8.0604766982292197</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="159.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="159.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1620,8 +1637,11 @@
       <c r="F9" s="1">
         <v>6.0307241719621398</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1634,60 +1654,82 @@
       <c r="F10" s="1">
         <v>13.140052281713499</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="1">
         <v>60.039101151044001</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="1">
         <v>69.056660892236096</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="159" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="1">
         <v>12.291001359411499</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="1">
         <v>2.74202018116396</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" ht="159" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="159" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="1">
         <v>9.3409946944558992</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="1">
         <v>7.83967960435265</v>
       </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1696,7 +1738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823F409E-BED1-4BED-A270-C2D15CB8042C}">
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1861,7 +1903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64667688-5B82-49DB-83F1-B2C271367828}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>